<commit_message>
Client name getter route fix
</commit_message>
<xml_diff>
--- a/backend/excel_files/boxes.xlsx
+++ b/backend/excel_files/boxes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilija\Desktop\RW_Destroy\backend\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C43221-57F8-4AEC-BCE3-46D5ADBDDA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4798433A-1422-44AD-AB4F-52451838A722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="24792" windowHeight="14976" xr2:uid="{06089E0E-4314-4FC5-9E03-EBF88954075E}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>Tura</t>
   </si>
   <si>
-    <t>Adiko</t>
-  </si>
-  <si>
     <t>026002680627</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>026002680631</t>
+  </si>
+  <si>
+    <t>Greba</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,10 +480,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="C2" s="2">
         <v>300</v>
@@ -491,10 +491,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2">
         <v>300</v>
@@ -502,10 +502,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <v>300</v>
@@ -513,10 +513,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>300</v>
@@ -524,10 +524,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2">
         <v>300</v>
@@ -535,10 +535,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2">
         <v>300</v>
@@ -546,10 +546,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2">
         <v>300</v>
@@ -557,10 +557,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2">
         <v>300</v>
@@ -568,10 +568,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2">
         <v>300</v>
@@ -579,10 +579,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2">
         <v>300</v>
@@ -590,10 +590,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2">
         <v>300</v>

</xml_diff>